<commit_message>
Timezone support with initialization
</commit_message>
<xml_diff>
--- a/demo/import.xlsx
+++ b/demo/import.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Temporary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick_tsai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B11AA4-53EE-4847-B7C2-EB39C2A2A8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -386,8 +387,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -426,17 +430,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -737,19 +743,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:100">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
@@ -1051,7 +1059,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:100" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:100" ht="32">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1064,520 +1072,523 @@
       <c r="D2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="6">
+        <v>43101.545138888891</v>
+      </c>
+      <c r="F2" s="2">
         <v>43101</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.38100000000000001</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:100">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:100">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:100">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:100">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:100">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:100">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:100">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:100">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:100">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:100">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:100">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:100">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:100">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:100">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1">
       <c r="A48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1">
       <c r="A49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1">
       <c r="A64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1">
       <c r="A65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1">
       <c r="A66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1">
       <c r="A67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1">
       <c r="A68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1">
       <c r="A69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1">
       <c r="A70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1">
       <c r="A71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1">
       <c r="A72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1">
       <c r="A73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1">
       <c r="A74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1">
       <c r="A75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1">
       <c r="A76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1">
       <c r="A77">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1">
       <c r="A78">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1">
       <c r="A79">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1">
       <c r="A80">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1">
       <c r="A81">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1">
       <c r="A82">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1">
       <c r="A83">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1">
       <c r="A84">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1">
       <c r="A85">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1">
       <c r="A86">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1">
       <c r="A87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1">
       <c r="A88">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1">
       <c r="A89">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1">
       <c r="A90">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1">
       <c r="A91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1">
       <c r="A92">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1">
       <c r="A93">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1">
       <c r="A94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1">
       <c r="A95">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1">
       <c r="A96">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1">
       <c r="A97">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1">
       <c r="A98">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1">
       <c r="A99">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1">
       <c r="A100">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1">
       <c r="A101">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="1">
-    <mergeCell ref="H2:I2"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>